<commit_message>
basline correction hassija dataset added
</commit_message>
<xml_diff>
--- a/Results/100K/all variations 100k.xlsx
+++ b/Results/100K/all variations 100k.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>With correct UUSIM (Pearson)</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>lam = 500 neigh=200 gnmf_components=50 gnmf_itr=1000</t>
+  </si>
+  <si>
+    <t>Neighbours</t>
+  </si>
+  <si>
+    <t>itr 10 (100K)</t>
+  </si>
+  <si>
+    <t>Lambda</t>
   </si>
 </sst>
 </file>
@@ -552,9 +561,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -876,15 +888,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GS15"/>
+  <dimension ref="A1:GS34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B30" sqref="A18:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:201" x14ac:dyDescent="0.25">
@@ -1977,6 +1990,108 @@
         <v>13</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>40</v>
+      </c>
+      <c r="B19">
+        <v>0.28272114799999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>80</v>
+      </c>
+      <c r="B20">
+        <v>0.27091421500000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>160</v>
+      </c>
+      <c r="B21">
+        <v>0.26678393099999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>160</v>
+      </c>
+      <c r="B22">
+        <v>0.26149692899999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>200</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.25672445300000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>240</v>
+      </c>
+      <c r="B24">
+        <v>0.26977474000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>100</v>
+      </c>
+      <c r="B27">
+        <v>0.28836862299999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>200</v>
+      </c>
+      <c r="B28">
+        <v>0.28272114799999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1000</v>
+      </c>
+      <c r="B29">
+        <v>0.26678393099999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2000</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.25672445300000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="34" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>